<commit_message>
Work through all vars
</commit_message>
<xml_diff>
--- a/data-raw/dictionary.xlsx
+++ b/data-raw/dictionary.xlsx
@@ -1550,7 +1550,7 @@
         <v>60</v>
       </c>
       <c r="D53" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E53" t="s">
         <v>9</v>
@@ -1567,7 +1567,7 @@
         <v>13</v>
       </c>
       <c r="D54" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E54" t="s">
         <v>9</v>
@@ -1584,7 +1584,7 @@
         <v>61</v>
       </c>
       <c r="D55" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E55" t="s">
         <v>9</v>
@@ -1601,7 +1601,7 @@
         <v>62</v>
       </c>
       <c r="D56" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E56" t="s">
         <v>9</v>
@@ -1618,7 +1618,7 @@
         <v>63</v>
       </c>
       <c r="D57" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E57" t="s">
         <v>9</v>
@@ -1635,7 +1635,7 @@
         <v>64</v>
       </c>
       <c r="D58" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E58" t="s">
         <v>9</v>
@@ -1652,7 +1652,7 @@
         <v>21</v>
       </c>
       <c r="D59" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E59" t="s">
         <v>9</v>
@@ -1669,7 +1669,7 @@
         <v>23</v>
       </c>
       <c r="D60" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E60" t="s">
         <v>9</v>
@@ -1686,7 +1686,7 @@
         <v>24</v>
       </c>
       <c r="D61" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E61" t="s">
         <v>9</v>
@@ -1703,7 +1703,7 @@
         <v>65</v>
       </c>
       <c r="D62" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E62" t="s">
         <v>9</v>
@@ -1720,7 +1720,7 @@
         <v>66</v>
       </c>
       <c r="D63" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E63" t="s">
         <v>9</v>
@@ -1737,7 +1737,7 @@
         <v>67</v>
       </c>
       <c r="D64" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E64" t="s">
         <v>9</v>
@@ -1771,7 +1771,7 @@
         <v>41</v>
       </c>
       <c r="D66" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E66" t="s">
         <v>9</v>
@@ -1805,7 +1805,7 @@
         <v>70</v>
       </c>
       <c r="D68" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E68" t="s">
         <v>9</v>
@@ -1822,7 +1822,7 @@
         <v>71</v>
       </c>
       <c r="D69" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E69" t="s">
         <v>9</v>
@@ -1839,7 +1839,7 @@
         <v>72</v>
       </c>
       <c r="D70" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E70" t="s">
         <v>9</v>
@@ -1856,7 +1856,7 @@
         <v>73</v>
       </c>
       <c r="D71" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E71" t="s">
         <v>9</v>
@@ -1873,7 +1873,7 @@
         <v>74</v>
       </c>
       <c r="D72" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E72" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Combine 4 resources into 1 dataset
</commit_message>
<xml_diff>
--- a/data-raw/dictionary.xlsx
+++ b/data-raw/dictionary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t xml:space="preserve">directory</t>
   </si>
@@ -237,6 +237,15 @@
   </si>
   <si>
     <t xml:space="preserve">vehicles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waste</t>
   </si>
   <si>
     <t xml:space="preserve">males</t>
@@ -1329,7 +1338,7 @@
         <v>49</v>
       </c>
       <c r="D40" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E40" t="s">
         <v>9</v>
@@ -1635,7 +1644,7 @@
         <v>64</v>
       </c>
       <c r="D58" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E58" t="s">
         <v>9</v>
@@ -1737,7 +1746,7 @@
         <v>67</v>
       </c>
       <c r="D64" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E64" t="s">
         <v>9</v>
@@ -1890,7 +1899,7 @@
         <v>75</v>
       </c>
       <c r="D73" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E73" t="s">
         <v>9</v>
@@ -1904,7 +1913,7 @@
         <v>59</v>
       </c>
       <c r="C74" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="D74" t="s">
         <v>12</v>
@@ -1921,7 +1930,7 @@
         <v>59</v>
       </c>
       <c r="C75" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="D75" t="s">
         <v>12</v>
@@ -1938,10 +1947,10 @@
         <v>59</v>
       </c>
       <c r="C76" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="D76" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E76" t="s">
         <v>9</v>
@@ -1952,13 +1961,13 @@
         <v>5</v>
       </c>
       <c r="B77" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C77" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="D77" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E77" t="s">
         <v>9</v>
@@ -1969,10 +1978,10 @@
         <v>5</v>
       </c>
       <c r="B78" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C78" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="D78" t="s">
         <v>12</v>
@@ -1986,13 +1995,13 @@
         <v>5</v>
       </c>
       <c r="B79" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C79" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="D79" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E79" t="s">
         <v>9</v>
@@ -2003,10 +2012,10 @@
         <v>5</v>
       </c>
       <c r="B80" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C80" t="s">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="D80" t="s">
         <v>8</v>
@@ -2020,7 +2029,7 @@
         <v>5</v>
       </c>
       <c r="B81" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C81" t="s">
         <v>80</v>
@@ -2037,7 +2046,7 @@
         <v>5</v>
       </c>
       <c r="B82" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C82" t="s">
         <v>81</v>
@@ -2054,13 +2063,13 @@
         <v>5</v>
       </c>
       <c r="B83" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C83" t="s">
         <v>82</v>
       </c>
       <c r="D83" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E83" t="s">
         <v>9</v>
@@ -2071,13 +2080,13 @@
         <v>5</v>
       </c>
       <c r="B84" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C84" t="s">
         <v>83</v>
       </c>
       <c r="D84" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E84" t="s">
         <v>9</v>
@@ -2088,7 +2097,7 @@
         <v>5</v>
       </c>
       <c r="B85" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C85" t="s">
         <v>84</v>
@@ -2105,13 +2114,13 @@
         <v>5</v>
       </c>
       <c r="B86" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C86" t="s">
         <v>85</v>
       </c>
       <c r="D86" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E86" t="s">
         <v>9</v>
@@ -2122,7 +2131,7 @@
         <v>5</v>
       </c>
       <c r="B87" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C87" t="s">
         <v>86</v>
@@ -2139,13 +2148,13 @@
         <v>5</v>
       </c>
       <c r="B88" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C88" t="s">
         <v>87</v>
       </c>
       <c r="D88" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E88" t="s">
         <v>9</v>
@@ -2156,7 +2165,7 @@
         <v>5</v>
       </c>
       <c r="B89" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C89" t="s">
         <v>88</v>
@@ -2173,7 +2182,7 @@
         <v>5</v>
       </c>
       <c r="B90" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C90" t="s">
         <v>89</v>
@@ -2190,13 +2199,13 @@
         <v>5</v>
       </c>
       <c r="B91" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C91" t="s">
         <v>90</v>
       </c>
       <c r="D91" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E91" t="s">
         <v>9</v>
@@ -2207,7 +2216,7 @@
         <v>5</v>
       </c>
       <c r="B92" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C92" t="s">
         <v>91</v>
@@ -2224,13 +2233,13 @@
         <v>5</v>
       </c>
       <c r="B93" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C93" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="D93" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E93" t="s">
         <v>9</v>
@@ -2241,10 +2250,10 @@
         <v>5</v>
       </c>
       <c r="B94" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C94" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="D94" t="s">
         <v>8</v>
@@ -2258,10 +2267,10 @@
         <v>5</v>
       </c>
       <c r="B95" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C95" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="D95" t="s">
         <v>8</v>
@@ -2275,13 +2284,13 @@
         <v>5</v>
       </c>
       <c r="B96" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C96" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="D96" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E96" t="s">
         <v>9</v>
@@ -2292,13 +2301,13 @@
         <v>5</v>
       </c>
       <c r="B97" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C97" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D97" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E97" t="s">
         <v>9</v>
@@ -2309,10 +2318,10 @@
         <v>5</v>
       </c>
       <c r="B98" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C98" t="s">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="D98" t="s">
         <v>8</v>
@@ -2326,10 +2335,10 @@
         <v>5</v>
       </c>
       <c r="B99" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C99" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D99" t="s">
         <v>8</v>
@@ -2343,13 +2352,13 @@
         <v>5</v>
       </c>
       <c r="B100" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C100" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D100" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E100" t="s">
         <v>9</v>
@@ -2360,10 +2369,10 @@
         <v>5</v>
       </c>
       <c r="B101" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C101" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="D101" t="s">
         <v>8</v>
@@ -2377,7 +2386,7 @@
         <v>5</v>
       </c>
       <c r="B102" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C102" t="s">
         <v>86</v>
@@ -2394,7 +2403,7 @@
         <v>5</v>
       </c>
       <c r="B103" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C103" t="s">
         <v>87</v>
@@ -2411,7 +2420,7 @@
         <v>5</v>
       </c>
       <c r="B104" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C104" t="s">
         <v>88</v>
@@ -2428,7 +2437,7 @@
         <v>5</v>
       </c>
       <c r="B105" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C105" t="s">
         <v>89</v>
@@ -2445,7 +2454,7 @@
         <v>5</v>
       </c>
       <c r="B106" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C106" t="s">
         <v>90</v>
@@ -2462,7 +2471,7 @@
         <v>5</v>
       </c>
       <c r="B107" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C107" t="s">
         <v>91</v>
@@ -2479,10 +2488,10 @@
         <v>5</v>
       </c>
       <c r="B108" t="s">
+        <v>95</v>
+      </c>
+      <c r="C108" t="s">
         <v>92</v>
-      </c>
-      <c r="C108" t="s">
-        <v>93</v>
       </c>
       <c r="D108" t="s">
         <v>8</v>
@@ -2496,13 +2505,13 @@
         <v>5</v>
       </c>
       <c r="B109" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C109" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D109" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E109" t="s">
         <v>9</v>
@@ -2513,13 +2522,13 @@
         <v>5</v>
       </c>
       <c r="B110" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C110" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D110" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E110" t="s">
         <v>9</v>
@@ -2530,13 +2539,13 @@
         <v>5</v>
       </c>
       <c r="B111" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C111" t="s">
         <v>96</v>
       </c>
       <c r="D111" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="E111" t="s">
         <v>9</v>
@@ -2547,13 +2556,13 @@
         <v>5</v>
       </c>
       <c r="B112" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C112" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D112" t="s">
-        <v>97</v>
+        <v>12</v>
       </c>
       <c r="E112" t="s">
         <v>9</v>
@@ -2564,10 +2573,10 @@
         <v>5</v>
       </c>
       <c r="B113" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C113" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D113" t="s">
         <v>12</v>
@@ -2581,13 +2590,13 @@
         <v>5</v>
       </c>
       <c r="B114" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C114" t="s">
+        <v>99</v>
+      </c>
+      <c r="D114" t="s">
         <v>100</v>
-      </c>
-      <c r="D114" t="s">
-        <v>12</v>
       </c>
       <c r="E114" t="s">
         <v>9</v>
@@ -2598,13 +2607,13 @@
         <v>5</v>
       </c>
       <c r="B115" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C115" t="s">
         <v>101</v>
       </c>
       <c r="D115" t="s">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="E115" t="s">
         <v>9</v>
@@ -2615,13 +2624,13 @@
         <v>5</v>
       </c>
       <c r="B116" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C116" t="s">
         <v>102</v>
       </c>
       <c r="D116" t="s">
-        <v>97</v>
+        <v>12</v>
       </c>
       <c r="E116" t="s">
         <v>9</v>
@@ -2632,13 +2641,13 @@
         <v>5</v>
       </c>
       <c r="B117" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C117" t="s">
         <v>103</v>
       </c>
       <c r="D117" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E117" t="s">
         <v>9</v>
@@ -2649,15 +2658,66 @@
         <v>5</v>
       </c>
       <c r="B118" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C118" t="s">
+        <v>104</v>
+      </c>
+      <c r="D118" t="s">
+        <v>12</v>
+      </c>
+      <c r="E118" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>5</v>
+      </c>
+      <c r="B119" t="s">
+        <v>95</v>
+      </c>
+      <c r="C119" t="s">
+        <v>105</v>
+      </c>
+      <c r="D119" t="s">
+        <v>100</v>
+      </c>
+      <c r="E119" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>5</v>
+      </c>
+      <c r="B120" t="s">
+        <v>95</v>
+      </c>
+      <c r="C120" t="s">
+        <v>106</v>
+      </c>
+      <c r="D120" t="s">
+        <v>8</v>
+      </c>
+      <c r="E120" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>5</v>
+      </c>
+      <c r="B121" t="s">
+        <v>95</v>
+      </c>
+      <c r="C121" t="s">
         <v>58</v>
       </c>
-      <c r="D118" t="s">
-        <v>12</v>
-      </c>
-      <c r="E118" t="s">
+      <c r="D121" t="s">
+        <v>12</v>
+      </c>
+      <c r="E121" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>